<commit_message>
Readme file and few adjustments on scripts
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF3DCE1-4F98-4452-8CB7-627EC9C0D51E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{8FF3DCE1-4F98-4452-8CB7-627EC9C0D51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FA93F2B-B36C-430D-A77A-4574A60D585A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="5820" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -21,6 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -646,6 +657,12 @@
     <t>fruit wine</t>
   </si>
   <si>
+    <t>AV491</t>
+  </si>
+  <si>
+    <t>dry legumes</t>
+  </si>
+  <si>
     <t>variable</t>
   </si>
   <si>
@@ -686,19 +703,13 @@
   </si>
   <si>
     <t>unknown</t>
-  </si>
-  <si>
-    <t>AV491</t>
-  </si>
-  <si>
-    <t>dry legumes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,7 +813,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1100,11 +1111,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="9"/>
     <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -1112,7 +1123,7 @@
     <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1140,7 +1151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1154,7 +1165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1168,7 +1179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1182,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1196,7 +1207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1210,7 +1221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1221,10 +1232,10 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1235,10 +1246,10 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1249,10 +1260,10 @@
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1263,10 +1274,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1277,10 +1288,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1291,10 +1302,10 @@
         <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1305,10 +1316,10 @@
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1319,10 +1330,10 @@
         <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1332,11 +1343,11 @@
       <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1346,11 +1357,11 @@
       <c r="C17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1360,11 +1371,11 @@
       <c r="C18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1374,11 +1385,11 @@
       <c r="C19" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1388,11 +1399,11 @@
       <c r="C20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1402,11 +1413,11 @@
       <c r="C21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1416,11 +1427,11 @@
       <c r="C22" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1430,11 +1441,11 @@
       <c r="C23" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1444,11 +1455,11 @@
       <c r="C24" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1458,11 +1469,11 @@
       <c r="C25" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1472,11 +1483,11 @@
       <c r="C26" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1486,11 +1497,11 @@
       <c r="C27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1500,11 +1511,11 @@
       <c r="C28" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1514,11 +1525,11 @@
       <c r="C29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1528,11 +1539,11 @@
       <c r="C30" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1542,11 +1553,11 @@
       <c r="C31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1556,11 +1567,11 @@
       <c r="C32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1570,11 +1581,11 @@
       <c r="C33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1584,11 +1595,11 @@
       <c r="C34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1598,11 +1609,11 @@
       <c r="C35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1612,11 +1623,11 @@
       <c r="C36" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1626,11 +1637,11 @@
       <c r="C37" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1640,11 +1651,11 @@
       <c r="C38" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1654,11 +1665,11 @@
       <c r="C39" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1668,11 +1679,11 @@
       <c r="C40" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1682,11 +1693,11 @@
       <c r="C41" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -1696,11 +1707,11 @@
       <c r="C42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1710,11 +1721,11 @@
       <c r="C43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1724,11 +1735,11 @@
       <c r="C44" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1738,11 +1749,11 @@
       <c r="C45" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1752,11 +1763,11 @@
       <c r="C46" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1766,11 +1777,11 @@
       <c r="C47" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -1780,11 +1791,11 @@
       <c r="C48" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1794,11 +1805,11 @@
       <c r="C49" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1808,11 +1819,11 @@
       <c r="C50" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1822,11 +1833,11 @@
       <c r="C51" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1836,11 +1847,11 @@
       <c r="C52" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -1850,11 +1861,11 @@
       <c r="C53" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D53" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -1864,11 +1875,11 @@
       <c r="C54" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D54" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1878,11 +1889,11 @@
       <c r="C55" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1892,11 +1903,11 @@
       <c r="C56" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1906,11 +1917,11 @@
       <c r="C57" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -1920,11 +1931,11 @@
       <c r="C58" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -1934,11 +1945,11 @@
       <c r="C59" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D59" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1948,11 +1959,11 @@
       <c r="C60" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1962,11 +1973,11 @@
       <c r="C61" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -1976,11 +1987,11 @@
       <c r="C62" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -1990,11 +2001,11 @@
       <c r="C63" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -2004,11 +2015,11 @@
       <c r="C64" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2018,11 +2029,11 @@
       <c r="C65" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2032,11 +2043,11 @@
       <c r="C66" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2046,11 +2057,11 @@
       <c r="C67" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2060,11 +2071,11 @@
       <c r="C68" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2074,11 +2085,11 @@
       <c r="C69" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D69" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2088,11 +2099,11 @@
       <c r="C70" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D70" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2102,11 +2113,11 @@
       <c r="C71" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="D71" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2116,11 +2127,11 @@
       <c r="C72" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2130,11 +2141,11 @@
       <c r="C73" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2144,11 +2155,11 @@
       <c r="C74" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2158,11 +2169,11 @@
       <c r="C75" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D75" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2172,11 +2183,11 @@
       <c r="C76" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D76" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2186,11 +2197,11 @@
       <c r="C77" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D77" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2200,11 +2211,11 @@
       <c r="C78" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D78" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2214,11 +2225,11 @@
       <c r="C79" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2228,11 +2239,11 @@
       <c r="C80" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D80" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2242,11 +2253,11 @@
       <c r="C81" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2256,11 +2267,11 @@
       <c r="C82" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D82" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D82" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2270,11 +2281,11 @@
       <c r="C83" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D83" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2284,11 +2295,11 @@
       <c r="C84" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D84" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2298,11 +2309,11 @@
       <c r="C85" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="D85" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2312,11 +2323,11 @@
       <c r="C86" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D86" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D86" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2326,11 +2337,11 @@
       <c r="C87" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D87" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2340,11 +2351,11 @@
       <c r="C88" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D88" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2354,11 +2365,11 @@
       <c r="C89" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2368,11 +2379,11 @@
       <c r="C90" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D90" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D90" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2382,14 +2393,14 @@
       <c r="C91" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D91" s="9" t="s">
-        <v>9</v>
+      <c r="D91" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="F91" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2399,11 +2410,11 @@
       <c r="C92" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D92" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2413,11 +2424,11 @@
       <c r="C93" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D93" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2427,11 +2438,11 @@
       <c r="C94" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D94" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2441,11 +2452,11 @@
       <c r="C95" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2455,11 +2466,11 @@
       <c r="C96" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="D96" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2469,11 +2480,11 @@
       <c r="C97" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D97" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2483,11 +2494,11 @@
       <c r="C98" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D98" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2497,11 +2508,11 @@
       <c r="C99" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D99" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2511,22 +2522,22 @@
       <c r="C100" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D100" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="9">
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>9</v>
+        <v>207</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2543,16 +2554,16 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2561,11 +2572,11 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="8" customFormat="1">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -2573,10 +2584,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -2584,10 +2595,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -2595,10 +2606,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2606,10 +2617,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -2617,10 +2628,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1">
       <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
@@ -2628,10 +2639,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1">
       <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
@@ -2639,10 +2650,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
@@ -2650,10 +2661,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -2661,10 +2672,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2672,10 +2683,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2683,10 +2694,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2694,1252 +2705,1252 @@
         <v>4</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2">
       <c r="A237" s="4"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2">
       <c r="A238" s="4"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2">
       <c r="A239" s="4"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2">
       <c r="A250" s="3"/>
       <c r="B250" s="5"/>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2">
       <c r="A251" s="3"/>
       <c r="B251" s="5"/>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2">
       <c r="A252" s="3"/>
       <c r="B252" s="5"/>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2">
       <c r="A253" s="3"/>
       <c r="B253" s="5"/>
     </row>
@@ -3950,18 +3961,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4202,7 +4201,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4211,40 +4210,26 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}"/>
 </file>
</xml_diff>

<commit_message>
inserted new line with additional variable "total energy intake" in DPE change decimal point from comma to point
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{8FF3DCE1-4F98-4452-8CB7-627EC9C0D51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FA93F2B-B36C-430D-A77A-4574A60D585A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B94C957C-0C91-4E78-94BE-CE725DF25482}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="5820" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="224">
   <si>
     <t>index</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>decimal</t>
+  </si>
+  <si>
+    <t>akcal</t>
+  </si>
+  <si>
+    <t>energy</t>
   </si>
   <si>
     <t>AV410</t>
@@ -709,7 +715,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,6 +744,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -759,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,6 +807,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -813,7 +828,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1109,13 +1124,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="9"/>
     <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -1123,7 +1138,7 @@
     <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +1152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1151,7 +1166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1165,7 +1180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1179,7 +1194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1193,7 +1208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1207,7 +1222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1221,11 +1236,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1235,7 +1250,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1249,7 +1264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1263,7 +1278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1277,7 +1292,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1291,7 +1306,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1305,7 +1320,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1319,7 +1334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1333,67 +1348,67 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -1403,11 +1418,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1417,7 +1432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1431,7 +1446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1445,7 +1460,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1459,7 +1474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1487,77 +1502,77 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="10" t="s">
         <v>62</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1571,7 +1586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1585,7 +1600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1613,21 +1628,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1641,11 +1656,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C38" s="9" t="s">
@@ -1655,7 +1670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1669,7 +1684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1683,7 +1698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1697,21 +1712,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="9" t="s">
         <v>88</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1725,7 +1740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1739,7 +1754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1753,7 +1768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1767,7 +1782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1781,21 +1796,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="3" t="s">
         <v>100</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1809,7 +1824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1823,7 +1838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1837,7 +1852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1851,35 +1866,35 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="9" t="s">
         <v>110</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="3" t="s">
         <v>112</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1893,7 +1908,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1907,7 +1922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1921,35 +1936,35 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="9" t="s">
         <v>120</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="3" t="s">
         <v>122</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1963,7 +1978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1977,63 +1992,63 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="9" t="s">
         <v>128</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="6" t="s">
         <v>130</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>64</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="6" t="s">
         <v>134</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2047,7 +2062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2061,7 +2076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2075,7 +2090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2089,7 +2104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2103,7 +2118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2117,7 +2132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2131,7 +2146,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2145,7 +2160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2159,7 +2174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2173,7 +2188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2187,7 +2202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2201,7 +2216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2215,7 +2230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2229,7 +2244,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2243,7 +2258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2257,7 +2272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2271,11 +2286,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>82</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="9" t="s">
         <v>169</v>
       </c>
       <c r="C83" s="9" t="s">
@@ -2285,7 +2300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2299,7 +2314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2313,11 +2328,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>85</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="3" t="s">
         <v>175</v>
       </c>
       <c r="C86" s="9" t="s">
@@ -2327,39 +2342,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="9" t="s">
         <v>178</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>87</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C89" s="9" t="s">
@@ -2369,7 +2384,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2383,7 +2398,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2396,25 +2411,25 @@
       <c r="D91" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F91" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="D92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92" t="s">
         <v>189</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2428,7 +2443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2442,7 +2457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2456,7 +2471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2470,7 +2485,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2484,7 +2499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2498,7 +2513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2512,7 +2527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2526,7 +2541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -2537,6 +2552,20 @@
         <v>207</v>
       </c>
       <c r="D101" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="9">
+        <v>101</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2554,16 +2583,16 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2572,11 +2601,11 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -2584,10 +2613,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -2595,10 +2624,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -2606,10 +2635,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2617,10 +2646,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -2628,10 +2657,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
@@ -2639,10 +2668,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
@@ -2650,10 +2679,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
@@ -2661,10 +2690,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -2672,10 +2701,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2683,10 +2712,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2694,10 +2723,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2705,1252 +2734,1252 @@
         <v>4</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="4"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="4"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="4"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="3"/>
       <c r="B250" s="5"/>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="3"/>
       <c r="B251" s="5"/>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="3"/>
       <c r="B252" s="5"/>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="3"/>
       <c r="B253" s="5"/>
     </row>
@@ -3961,6 +3990,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4201,35 +4251,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to P1 documents and scripts
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B94C957C-0C91-4E78-94BE-CE725DF25482}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666ACD5-488A-46B5-92B7-740638CFBDBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -21,17 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -51,9 +40,6 @@
     <t>valueType</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>ID of the participant</t>
   </si>
   <si>
@@ -709,6 +695,9 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>A_ID</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1116,7 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,13 +1146,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,13 +1160,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,13 +1174,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,13 +1188,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1213,13 +1202,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1227,13 +1216,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,13 +1230,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,13 +1244,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1269,13 +1258,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,13 +1272,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,13 +1286,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,13 +1300,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,13 +1314,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1339,13 +1328,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,13 +1342,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,13 +1356,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1381,13 +1370,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,13 +1384,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1409,13 +1398,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1423,13 +1412,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>46</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,13 +1426,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1451,13 +1440,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>50</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1465,13 +1454,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1479,13 +1468,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1493,13 +1482,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1507,13 +1496,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>58</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,13 +1510,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1535,13 +1524,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1549,13 +1538,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,13 +1552,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,13 +1566,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,13 +1580,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,13 +1594,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1619,13 +1608,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1633,13 +1622,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1647,13 +1636,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>78</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1661,13 +1650,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,13 +1664,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>82</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1689,13 +1678,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1703,13 +1692,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,13 +1706,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>88</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1731,13 +1720,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1745,13 +1734,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,13 +1748,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1773,13 +1762,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1787,13 +1776,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1801,13 +1790,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="D48" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1815,13 +1804,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>102</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,13 +1818,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>104</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1843,13 +1832,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,13 +1846,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1871,13 +1860,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>110</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1885,13 +1874,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="D54" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1899,13 +1888,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="9" t="s">
-        <v>114</v>
-      </c>
       <c r="D55" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,13 +1902,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>116</v>
-      </c>
       <c r="D56" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,13 +1916,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="9" t="s">
-        <v>118</v>
-      </c>
       <c r="D57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,13 +1930,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>120</v>
-      </c>
       <c r="D58" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,13 +1944,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,13 +1958,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="D60" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1983,13 +1972,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C61" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="9" t="s">
-        <v>126</v>
-      </c>
       <c r="D61" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1997,13 +1986,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>128</v>
-      </c>
       <c r="D62" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2011,13 +2000,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="6" t="s">
-        <v>130</v>
-      </c>
       <c r="D63" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2025,13 +2014,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="D64" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2039,13 +2028,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="6" t="s">
-        <v>134</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2053,13 +2042,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>136</v>
-      </c>
       <c r="D66" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2067,13 +2056,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C67" s="9" t="s">
-        <v>138</v>
-      </c>
       <c r="D67" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2081,13 +2070,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>140</v>
-      </c>
       <c r="D68" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,13 +2084,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C69" s="9" t="s">
-        <v>142</v>
-      </c>
       <c r="D69" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2109,13 +2098,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>144</v>
-      </c>
       <c r="D70" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2123,13 +2112,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="9" t="s">
-        <v>146</v>
-      </c>
       <c r="D71" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2137,13 +2126,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>148</v>
-      </c>
       <c r="D72" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2151,13 +2140,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C73" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="D73" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2165,13 +2154,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C74" s="9" t="s">
-        <v>152</v>
-      </c>
       <c r="D74" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,13 +2168,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C75" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="D75" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2193,13 +2182,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>156</v>
-      </c>
       <c r="D76" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2207,13 +2196,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C77" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C77" s="9" t="s">
-        <v>158</v>
-      </c>
       <c r="D77" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,13 +2210,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C78" s="9" t="s">
-        <v>160</v>
-      </c>
       <c r="D78" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2235,13 +2224,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C79" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="D79" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2249,13 +2238,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C80" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C80" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="D80" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2263,13 +2252,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C81" s="9" t="s">
-        <v>166</v>
-      </c>
       <c r="D81" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2277,13 +2266,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C82" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C82" s="9" t="s">
-        <v>168</v>
-      </c>
       <c r="D82" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2291,13 +2280,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C83" s="9" t="s">
-        <v>170</v>
-      </c>
       <c r="D83" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2305,13 +2294,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C84" s="9" t="s">
-        <v>172</v>
-      </c>
       <c r="D84" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2319,13 +2308,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C85" s="9" t="s">
-        <v>174</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2333,13 +2322,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C86" s="9" t="s">
-        <v>176</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,13 +2336,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C87" s="9" t="s">
-        <v>178</v>
-      </c>
       <c r="D87" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2361,13 +2350,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="D88" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2375,13 +2364,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="9" t="s">
-        <v>182</v>
-      </c>
       <c r="D89" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2389,13 +2378,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C90" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C90" s="9" t="s">
-        <v>184</v>
-      </c>
       <c r="D90" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2403,13 +2392,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C91" s="9" t="s">
-        <v>186</v>
-      </c>
       <c r="D91" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2417,16 +2406,16 @@
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="D92" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F92" t="s">
         <v>188</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F92" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2434,13 +2423,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C93" s="9" t="s">
-        <v>191</v>
-      </c>
       <c r="D93" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2448,13 +2437,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C94" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="D94" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2462,13 +2451,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C95" s="9" t="s">
-        <v>195</v>
-      </c>
       <c r="D95" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2476,13 +2465,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C96" s="9" t="s">
-        <v>197</v>
-      </c>
       <c r="D96" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2490,13 +2479,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="C97" s="9" t="s">
-        <v>199</v>
-      </c>
       <c r="D97" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,13 +2493,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C98" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C98" s="9" t="s">
-        <v>201</v>
-      </c>
       <c r="D98" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2518,13 +2507,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C99" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C99" s="9" t="s">
-        <v>203</v>
-      </c>
       <c r="D99" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2532,13 +2521,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C100" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C100" s="9" t="s">
-        <v>205</v>
-      </c>
       <c r="D100" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2546,13 +2535,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C101" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C101" s="9" t="s">
-        <v>207</v>
-      </c>
       <c r="D101" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2560,13 +2549,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C102" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="C102" s="9" t="s">
-        <v>209</v>
-      </c>
       <c r="D102" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2592,7 +2581,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2601,140 +2590,140 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="12">
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="12">
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="12">
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="12">
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="12">
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="12">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="12">
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="12">
         <v>3</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="12">
         <v>4</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3990,27 +3979,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4251,10 +4219,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4277,20 +4277,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added akcal to the list of variables in DD_KORA_S1_P1
changed ID variable into a_id in DPE_KORA_S1_P1
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666ACD5-488A-46B5-92B7-740638CFBDBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{355F4338-A502-405F-B1B3-778194FD8D2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="219">
   <si>
     <t>index</t>
   </si>
@@ -43,9 +43,6 @@
     <t>ID of the participant</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>acsex</t>
   </si>
   <si>
@@ -82,629 +79,617 @@
     <t>decimal</t>
   </si>
   <si>
+    <t>AV410</t>
+  </si>
+  <si>
+    <t>potatoes</t>
+  </si>
+  <si>
+    <t>AV420</t>
+  </si>
+  <si>
+    <t>potato products</t>
+  </si>
+  <si>
+    <t>AV431</t>
+  </si>
+  <si>
+    <t>cauliflower</t>
+  </si>
+  <si>
+    <t>AV433</t>
+  </si>
+  <si>
+    <t>other cabbage</t>
+  </si>
+  <si>
+    <t>AV440</t>
+  </si>
+  <si>
+    <t>leafy and stem vegetables</t>
+  </si>
+  <si>
+    <t>AV451</t>
+  </si>
+  <si>
+    <t>tomatoes</t>
+  </si>
+  <si>
+    <t>AV455</t>
+  </si>
+  <si>
+    <t>cucumbers</t>
+  </si>
+  <si>
+    <t>AV459</t>
+  </si>
+  <si>
+    <t>other fruit vegetables</t>
+  </si>
+  <si>
+    <t>AV461</t>
+  </si>
+  <si>
+    <t>onion vegetables</t>
+  </si>
+  <si>
+    <t>AV465</t>
+  </si>
+  <si>
+    <t>carrots</t>
+  </si>
+  <si>
+    <t>AV469</t>
+  </si>
+  <si>
+    <t>other fresh vegetables</t>
+  </si>
+  <si>
+    <t>AV470</t>
+  </si>
+  <si>
+    <t>frozen vegetables</t>
+  </si>
+  <si>
+    <t>AV480</t>
+  </si>
+  <si>
+    <t>canned vegetables</t>
+  </si>
+  <si>
+    <t>AV499</t>
+  </si>
+  <si>
+    <t>other vegetable products</t>
+  </si>
+  <si>
+    <t>AV310</t>
+  </si>
+  <si>
+    <t>fruit without specification</t>
+  </si>
+  <si>
+    <t>AV311</t>
+  </si>
+  <si>
+    <t>apples</t>
+  </si>
+  <si>
+    <t>AV315</t>
+  </si>
+  <si>
+    <t>other pome fruits</t>
+  </si>
+  <si>
+    <t>AV321</t>
+  </si>
+  <si>
+    <t>peaches</t>
+  </si>
+  <si>
+    <t>AV323</t>
+  </si>
+  <si>
+    <t>cherries</t>
+  </si>
+  <si>
+    <t>AV325</t>
+  </si>
+  <si>
+    <t>other stone fruits</t>
+  </si>
+  <si>
+    <t>AV331</t>
+  </si>
+  <si>
+    <t>strawberries</t>
+  </si>
+  <si>
+    <t>AV334</t>
+  </si>
+  <si>
+    <t>other berries</t>
+  </si>
+  <si>
+    <t>AV337</t>
+  </si>
+  <si>
+    <t>grapes</t>
+  </si>
+  <si>
+    <t>AV341</t>
+  </si>
+  <si>
+    <t>oranges, mandarins</t>
+  </si>
+  <si>
+    <t>AV343</t>
+  </si>
+  <si>
+    <t>grapefruits</t>
+  </si>
+  <si>
+    <t>AV344</t>
+  </si>
+  <si>
+    <t>other citrus fruits</t>
+  </si>
+  <si>
+    <t>AV345</t>
+  </si>
+  <si>
+    <t>bananas</t>
+  </si>
+  <si>
+    <t>AV346</t>
+  </si>
+  <si>
+    <t>other tropical fruits</t>
+  </si>
+  <si>
+    <t>AV351</t>
+  </si>
+  <si>
+    <t>nuts</t>
+  </si>
+  <si>
+    <t>AV357</t>
+  </si>
+  <si>
+    <t>dried fruit</t>
+  </si>
+  <si>
+    <t>AV360</t>
+  </si>
+  <si>
+    <t>canned fruit</t>
+  </si>
+  <si>
+    <t>AV370</t>
+  </si>
+  <si>
+    <t>frozen fruit</t>
+  </si>
+  <si>
+    <t>AV390</t>
+  </si>
+  <si>
+    <t>other processed fruit</t>
+  </si>
+  <si>
+    <t>AV210</t>
+  </si>
+  <si>
+    <t>drinking milk</t>
+  </si>
+  <si>
+    <t>AV220</t>
+  </si>
+  <si>
+    <t>condensed milk or powder</t>
+  </si>
+  <si>
+    <t>AV231</t>
+  </si>
+  <si>
+    <t>cream</t>
+  </si>
+  <si>
+    <t>AV232</t>
+  </si>
+  <si>
+    <t>yogurt, soured milk</t>
+  </si>
+  <si>
+    <t>AV233</t>
+  </si>
+  <si>
+    <t>other dairy products</t>
+  </si>
+  <si>
+    <t>AV245</t>
+  </si>
+  <si>
+    <t>fresh cheese, curd</t>
+  </si>
+  <si>
+    <t>AV248</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>AV711</t>
+  </si>
+  <si>
+    <t>Wheat flour</t>
+  </si>
+  <si>
+    <t>AV715</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>AV731</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>AV719</t>
+  </si>
+  <si>
+    <t>Products from other cereals</t>
+  </si>
+  <si>
+    <t>AV511</t>
+  </si>
+  <si>
+    <t>White bread</t>
+  </si>
+  <si>
+    <t>AV512</t>
+  </si>
+  <si>
+    <t>Brown bread</t>
+  </si>
+  <si>
+    <t>AV517</t>
+  </si>
+  <si>
+    <t>Other bread</t>
+  </si>
+  <si>
+    <t>AV515</t>
+  </si>
+  <si>
+    <t>Crisp bread</t>
+  </si>
+  <si>
+    <t>AV540</t>
+  </si>
+  <si>
+    <t>Fine bakery products</t>
+  </si>
+  <si>
+    <t>AV111</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>AV112</t>
+  </si>
+  <si>
+    <t>Veal</t>
+  </si>
+  <si>
+    <t>AV113</t>
+  </si>
+  <si>
+    <t>Pork meat</t>
+  </si>
+  <si>
+    <t>AV115</t>
+  </si>
+  <si>
+    <t>Sheep or goat meat</t>
+  </si>
+  <si>
+    <t>AV117</t>
+  </si>
+  <si>
+    <t>Game meat</t>
+  </si>
+  <si>
+    <t>AV119</t>
+  </si>
+  <si>
+    <t>other meat</t>
+  </si>
+  <si>
+    <t>AV120</t>
+  </si>
+  <si>
+    <t>Poultry meat</t>
+  </si>
+  <si>
+    <t>AV131</t>
+  </si>
+  <si>
+    <t>Minced meat</t>
+  </si>
+  <si>
+    <t>AV135</t>
+  </si>
+  <si>
+    <t>Animal offal</t>
+  </si>
+  <si>
+    <t>AV141</t>
+  </si>
+  <si>
+    <t>Sausage</t>
+  </si>
+  <si>
+    <t>AV145</t>
+  </si>
+  <si>
+    <t>Ham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV147 </t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>AV150</t>
+  </si>
+  <si>
+    <t>canned, frozen meat or meat products</t>
+  </si>
+  <si>
+    <t>AV160</t>
+  </si>
+  <si>
+    <t>other meat products</t>
+  </si>
+  <si>
+    <t>AV170</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>AV180</t>
+  </si>
+  <si>
+    <t>canned fish</t>
+  </si>
+  <si>
+    <t>AV190</t>
+  </si>
+  <si>
+    <t>other fish products</t>
+  </si>
+  <si>
+    <t>AV250</t>
+  </si>
+  <si>
+    <t>fresh eggs</t>
+  </si>
+  <si>
+    <t>AV255</t>
+  </si>
+  <si>
+    <t>egg products</t>
+  </si>
+  <si>
+    <t>AV270</t>
+  </si>
+  <si>
+    <t>butter</t>
+  </si>
+  <si>
+    <t>AV291</t>
+  </si>
+  <si>
+    <t>margarine</t>
+  </si>
+  <si>
+    <t>AV293</t>
+  </si>
+  <si>
+    <t>vegetable edible oils</t>
+  </si>
+  <si>
+    <t>AV295</t>
+  </si>
+  <si>
+    <t>other edible oils</t>
+  </si>
+  <si>
+    <t>AV610</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>AV681</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>AV684</t>
+  </si>
+  <si>
+    <t>Jam</t>
+  </si>
+  <si>
+    <t>AV687</t>
+  </si>
+  <si>
+    <t>Other sweet spreads</t>
+  </si>
+  <si>
+    <t>AV620</t>
+  </si>
+  <si>
+    <t>cacao products</t>
+  </si>
+  <si>
+    <t>AV630</t>
+  </si>
+  <si>
+    <t>chocolate products</t>
+  </si>
+  <si>
+    <t>AV650</t>
+  </si>
+  <si>
+    <t>confectionary</t>
+  </si>
+  <si>
+    <t>AV670</t>
+  </si>
+  <si>
+    <t>all ice cream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV570 </t>
+  </si>
+  <si>
+    <t>long-life baked goods</t>
+  </si>
+  <si>
+    <t>AV810</t>
+  </si>
+  <si>
+    <t>fruit/vegetable juice</t>
+  </si>
+  <si>
+    <t>AV821</t>
+  </si>
+  <si>
+    <t>table water</t>
+  </si>
+  <si>
+    <t>AV825</t>
+  </si>
+  <si>
+    <t>caffeinated lemonade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AV829</t>
+  </si>
+  <si>
+    <t>other soft drinks</t>
+  </si>
+  <si>
+    <t>AV841</t>
+  </si>
+  <si>
+    <t>roasted coffee</t>
+  </si>
+  <si>
+    <t>AV845</t>
+  </si>
+  <si>
+    <t>coffee extracts</t>
+  </si>
+  <si>
+    <t>AV850</t>
+  </si>
+  <si>
+    <t>tea</t>
+  </si>
+  <si>
+    <t>AV860</t>
+  </si>
+  <si>
+    <t>spirits</t>
+  </si>
+  <si>
+    <t>AV870</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>AV881</t>
+  </si>
+  <si>
+    <t>grape wine</t>
+  </si>
+  <si>
+    <t>AV885</t>
+  </si>
+  <si>
+    <t>grape sparkling wine</t>
+  </si>
+  <si>
+    <t>AV889</t>
+  </si>
+  <si>
+    <t>fruit wine</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>technical/professional school completed</t>
+  </si>
+  <si>
+    <t>secondary school</t>
+  </si>
+  <si>
+    <t>longer education (incl. university)</t>
+  </si>
+  <si>
+    <t>never</t>
+  </si>
+  <si>
+    <t>former</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>a_id</t>
+  </si>
+  <si>
+    <t>AV491</t>
+  </si>
+  <si>
+    <t>dry legumes</t>
+  </si>
+  <si>
+    <t>primary school completed</t>
+  </si>
+  <si>
     <t>akcal</t>
   </si>
   <si>
     <t>energy</t>
-  </si>
-  <si>
-    <t>AV410</t>
-  </si>
-  <si>
-    <t>potatoes</t>
-  </si>
-  <si>
-    <t>AV420</t>
-  </si>
-  <si>
-    <t>potato products</t>
-  </si>
-  <si>
-    <t>AV431</t>
-  </si>
-  <si>
-    <t>cauliflower</t>
-  </si>
-  <si>
-    <t>AV433</t>
-  </si>
-  <si>
-    <t>other cabbage</t>
-  </si>
-  <si>
-    <t>AV440</t>
-  </si>
-  <si>
-    <t>leafy and stem vegetables</t>
-  </si>
-  <si>
-    <t>AV451</t>
-  </si>
-  <si>
-    <t>tomatoes</t>
-  </si>
-  <si>
-    <t>AV455</t>
-  </si>
-  <si>
-    <t>cucumbers</t>
-  </si>
-  <si>
-    <t>AV459</t>
-  </si>
-  <si>
-    <t>other fruit vegetables</t>
-  </si>
-  <si>
-    <t>AV461</t>
-  </si>
-  <si>
-    <t>onion vegetables</t>
-  </si>
-  <si>
-    <t>AV465</t>
-  </si>
-  <si>
-    <t>carrots</t>
-  </si>
-  <si>
-    <t>AV469</t>
-  </si>
-  <si>
-    <t>other fresh vegetables</t>
-  </si>
-  <si>
-    <t>AV470</t>
-  </si>
-  <si>
-    <t>frozen vegetables</t>
-  </si>
-  <si>
-    <t>AV480</t>
-  </si>
-  <si>
-    <t>canned vegetables</t>
-  </si>
-  <si>
-    <t>AV499</t>
-  </si>
-  <si>
-    <t>other vegetable products</t>
-  </si>
-  <si>
-    <t>AV310</t>
-  </si>
-  <si>
-    <t>fruit without specification</t>
-  </si>
-  <si>
-    <t>AV311</t>
-  </si>
-  <si>
-    <t>apples</t>
-  </si>
-  <si>
-    <t>AV315</t>
-  </si>
-  <si>
-    <t>other pome fruits</t>
-  </si>
-  <si>
-    <t>AV321</t>
-  </si>
-  <si>
-    <t>peaches</t>
-  </si>
-  <si>
-    <t>AV323</t>
-  </si>
-  <si>
-    <t>cherries</t>
-  </si>
-  <si>
-    <t>AV325</t>
-  </si>
-  <si>
-    <t>other stone fruits</t>
-  </si>
-  <si>
-    <t>AV331</t>
-  </si>
-  <si>
-    <t>strawberries</t>
-  </si>
-  <si>
-    <t>AV334</t>
-  </si>
-  <si>
-    <t>other berries</t>
-  </si>
-  <si>
-    <t>AV337</t>
-  </si>
-  <si>
-    <t>grapes</t>
-  </si>
-  <si>
-    <t>AV341</t>
-  </si>
-  <si>
-    <t>oranges, mandarins</t>
-  </si>
-  <si>
-    <t>AV343</t>
-  </si>
-  <si>
-    <t>grapefruits</t>
-  </si>
-  <si>
-    <t>AV344</t>
-  </si>
-  <si>
-    <t>other citrus fruits</t>
-  </si>
-  <si>
-    <t>AV345</t>
-  </si>
-  <si>
-    <t>bananas</t>
-  </si>
-  <si>
-    <t>AV346</t>
-  </si>
-  <si>
-    <t>other tropical fruits</t>
-  </si>
-  <si>
-    <t>AV351</t>
-  </si>
-  <si>
-    <t>nuts</t>
-  </si>
-  <si>
-    <t>AV357</t>
-  </si>
-  <si>
-    <t>dried fruit</t>
-  </si>
-  <si>
-    <t>AV360</t>
-  </si>
-  <si>
-    <t>canned fruit</t>
-  </si>
-  <si>
-    <t>AV370</t>
-  </si>
-  <si>
-    <t>frozen fruit</t>
-  </si>
-  <si>
-    <t>AV390</t>
-  </si>
-  <si>
-    <t>other processed fruit</t>
-  </si>
-  <si>
-    <t>AV210</t>
-  </si>
-  <si>
-    <t>drinking milk</t>
-  </si>
-  <si>
-    <t>AV220</t>
-  </si>
-  <si>
-    <t>condensed milk or powder</t>
-  </si>
-  <si>
-    <t>AV231</t>
-  </si>
-  <si>
-    <t>cream</t>
-  </si>
-  <si>
-    <t>AV232</t>
-  </si>
-  <si>
-    <t>yogurt, soured milk</t>
-  </si>
-  <si>
-    <t>AV233</t>
-  </si>
-  <si>
-    <t>other dairy products</t>
-  </si>
-  <si>
-    <t>AV245</t>
-  </si>
-  <si>
-    <t>fresh cheese, curd</t>
-  </si>
-  <si>
-    <t>AV248</t>
-  </si>
-  <si>
-    <t>cheese</t>
-  </si>
-  <si>
-    <t>AV711</t>
-  </si>
-  <si>
-    <t>Wheat flour</t>
-  </si>
-  <si>
-    <t>AV715</t>
-  </si>
-  <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>AV731</t>
-  </si>
-  <si>
-    <t>Pasta</t>
-  </si>
-  <si>
-    <t>AV719</t>
-  </si>
-  <si>
-    <t>Products from other cereals</t>
-  </si>
-  <si>
-    <t>AV511</t>
-  </si>
-  <si>
-    <t>White bread</t>
-  </si>
-  <si>
-    <t>AV512</t>
-  </si>
-  <si>
-    <t>Brown bread</t>
-  </si>
-  <si>
-    <t>AV517</t>
-  </si>
-  <si>
-    <t>Other bread</t>
-  </si>
-  <si>
-    <t>AV515</t>
-  </si>
-  <si>
-    <t>Crisp bread</t>
-  </si>
-  <si>
-    <t>AV540</t>
-  </si>
-  <si>
-    <t>Fine bakery products</t>
-  </si>
-  <si>
-    <t>AV111</t>
-  </si>
-  <si>
-    <t>Beef</t>
-  </si>
-  <si>
-    <t>AV112</t>
-  </si>
-  <si>
-    <t>Veal</t>
-  </si>
-  <si>
-    <t>AV113</t>
-  </si>
-  <si>
-    <t>Pork meat</t>
-  </si>
-  <si>
-    <t>AV115</t>
-  </si>
-  <si>
-    <t>Sheep or goat meat</t>
-  </si>
-  <si>
-    <t>AV117</t>
-  </si>
-  <si>
-    <t>Game meat</t>
-  </si>
-  <si>
-    <t>AV119</t>
-  </si>
-  <si>
-    <t>other meat</t>
-  </si>
-  <si>
-    <t>AV120</t>
-  </si>
-  <si>
-    <t>Poultry meat</t>
-  </si>
-  <si>
-    <t>AV131</t>
-  </si>
-  <si>
-    <t>Minced meat</t>
-  </si>
-  <si>
-    <t>AV135</t>
-  </si>
-  <si>
-    <t>Animal offal</t>
-  </si>
-  <si>
-    <t>AV141</t>
-  </si>
-  <si>
-    <t>Sausage</t>
-  </si>
-  <si>
-    <t>AV145</t>
-  </si>
-  <si>
-    <t>Ham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AV147 </t>
-  </si>
-  <si>
-    <t>Bacon</t>
-  </si>
-  <si>
-    <t>AV150</t>
-  </si>
-  <si>
-    <t>canned, frozen meat or meat products</t>
-  </si>
-  <si>
-    <t>AV160</t>
-  </si>
-  <si>
-    <t>other meat products</t>
-  </si>
-  <si>
-    <t>AV170</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-  <si>
-    <t>AV180</t>
-  </si>
-  <si>
-    <t>canned fish</t>
-  </si>
-  <si>
-    <t>AV190</t>
-  </si>
-  <si>
-    <t>other fish products</t>
-  </si>
-  <si>
-    <t>AV250</t>
-  </si>
-  <si>
-    <t>fresh eggs</t>
-  </si>
-  <si>
-    <t>AV255</t>
-  </si>
-  <si>
-    <t>egg products</t>
-  </si>
-  <si>
-    <t>AV270</t>
-  </si>
-  <si>
-    <t>butter</t>
-  </si>
-  <si>
-    <t>AV291</t>
-  </si>
-  <si>
-    <t>margarine</t>
-  </si>
-  <si>
-    <t>AV293</t>
-  </si>
-  <si>
-    <t>vegetable edible oils</t>
-  </si>
-  <si>
-    <t>AV295</t>
-  </si>
-  <si>
-    <t>other edible oils</t>
-  </si>
-  <si>
-    <t>AV610</t>
-  </si>
-  <si>
-    <t>sugar</t>
-  </si>
-  <si>
-    <t>AV681</t>
-  </si>
-  <si>
-    <t>Honey</t>
-  </si>
-  <si>
-    <t>AV684</t>
-  </si>
-  <si>
-    <t>Jam</t>
-  </si>
-  <si>
-    <t>AV687</t>
-  </si>
-  <si>
-    <t>Other sweet spreads</t>
-  </si>
-  <si>
-    <t>AV620</t>
-  </si>
-  <si>
-    <t>cacao products</t>
-  </si>
-  <si>
-    <t>AV630</t>
-  </si>
-  <si>
-    <t>chocolate products</t>
-  </si>
-  <si>
-    <t>AV650</t>
-  </si>
-  <si>
-    <t>confectionary</t>
-  </si>
-  <si>
-    <t>AV670</t>
-  </si>
-  <si>
-    <t>all ice cream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AV570 </t>
-  </si>
-  <si>
-    <t>long-life baked goods</t>
-  </si>
-  <si>
-    <t>AV810</t>
-  </si>
-  <si>
-    <t>fruit/vegetable juice</t>
-  </si>
-  <si>
-    <t>AV821</t>
-  </si>
-  <si>
-    <t>table water</t>
-  </si>
-  <si>
-    <t>AV825</t>
-  </si>
-  <si>
-    <t>caffeinated lemonade</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>AV829</t>
-  </si>
-  <si>
-    <t>other soft drinks</t>
-  </si>
-  <si>
-    <t>AV841</t>
-  </si>
-  <si>
-    <t>roasted coffee</t>
-  </si>
-  <si>
-    <t>AV845</t>
-  </si>
-  <si>
-    <t>coffee extracts</t>
-  </si>
-  <si>
-    <t>AV850</t>
-  </si>
-  <si>
-    <t>tea</t>
-  </si>
-  <si>
-    <t>AV860</t>
-  </si>
-  <si>
-    <t>spirits</t>
-  </si>
-  <si>
-    <t>AV870</t>
-  </si>
-  <si>
-    <t>beer</t>
-  </si>
-  <si>
-    <t>AV881</t>
-  </si>
-  <si>
-    <t>grape wine</t>
-  </si>
-  <si>
-    <t>AV885</t>
-  </si>
-  <si>
-    <t>grape sparkling wine</t>
-  </si>
-  <si>
-    <t>AV889</t>
-  </si>
-  <si>
-    <t>fruit wine</t>
-  </si>
-  <si>
-    <t>AV491</t>
-  </si>
-  <si>
-    <t>dry legumes</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>primary school completed</t>
-  </si>
-  <si>
-    <t>technical/professional school completed</t>
-  </si>
-  <si>
-    <t>secondary school</t>
-  </si>
-  <si>
-    <t>longer education (incl. university)</t>
-  </si>
-  <si>
-    <t>not specified</t>
-  </si>
-  <si>
-    <t>never</t>
-  </si>
-  <si>
-    <t>former</t>
-  </si>
-  <si>
-    <t>current</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>A_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,12 +718,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -760,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,9 +774,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,14 +1092,14 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="9"/>
-    <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="9" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="9" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
@@ -1146,13 +1122,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,13 +1136,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,13 +1150,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,13 +1164,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,13 +1178,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,27 +1192,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>18</v>
+      <c r="B8" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>218</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,13 +1220,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,13 +1234,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,13 +1248,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,13 +1262,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,13 +1276,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,13 +1290,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,13 +1304,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,13 +1318,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,13 +1332,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,13 +1346,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,13 +1360,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,13 +1374,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,27 +1388,27 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+      <c r="B22" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,13 +1416,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,13 +1430,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1468,13 +1444,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,13 +1458,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,13 +1472,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,13 +1486,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1524,13 +1500,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,13 +1514,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,13 +1528,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,13 +1542,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1580,13 +1556,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1594,13 +1570,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,13 +1584,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1622,27 +1598,27 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>77</v>
+      <c r="B37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,27 +1626,27 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>80</v>
+      <c r="B39" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,13 +1654,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1692,13 +1668,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1706,13 +1682,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,13 +1696,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,13 +1710,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,13 +1724,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1762,13 +1738,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1776,13 +1752,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,13 +1766,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1804,13 +1780,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1818,13 +1794,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1832,13 +1808,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1846,13 +1822,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1860,13 +1836,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1874,13 +1850,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,13 +1864,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,13 +1878,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,13 +1892,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,13 +1906,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1944,13 +1920,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1958,13 +1934,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>123</v>
+        <v>117</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,13 +1948,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,13 +1962,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2000,13 +1976,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,13 +1990,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,27 +2004,27 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
-      <c r="B66" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>135</v>
+      <c r="B66" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2056,13 +2032,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2070,13 +2046,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,13 +2060,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2098,13 +2074,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,13 +2088,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,13 +2102,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2140,13 +2116,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,13 +2130,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,13 +2144,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2182,13 +2158,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2196,13 +2172,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2210,13 +2186,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,13 +2200,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2238,13 +2214,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2252,13 +2228,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2266,13 +2242,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2280,27 +2256,27 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>170</v>
+      <c r="B84" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2308,13 +2284,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2322,27 +2298,27 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
-      <c r="B87" s="9" t="s">
-        <v>176</v>
+      <c r="B87" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2350,41 +2326,41 @@
         <v>87</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>181</v>
+      <c r="B89" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
-      <c r="B90" s="9" t="s">
-        <v>182</v>
+      <c r="B90" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2392,13 +2368,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2406,16 +2382,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" t="s">
-        <v>188</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2423,13 +2396,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="F93" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2437,13 +2413,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2451,13 +2427,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2465,13 +2441,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2479,13 +2455,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2493,13 +2469,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2507,13 +2483,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2521,13 +2497,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2535,13 +2511,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2549,13 +2525,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2566,22 +2542,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2590,141 +2564,121 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="12">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="C8" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="12">
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="12">
-        <v>4</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="12">
-        <v>5</v>
-      </c>
       <c r="C9" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="12">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="12">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="12">
-        <v>4</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>222</v>
-      </c>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -2871,25 +2825,25 @@
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+      <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+      <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+      <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+      <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -3471,25 +3425,25 @@
       <c r="D137" s="8"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="3"/>
+      <c r="A138" s="9"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="3"/>
+      <c r="A139" s="9"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="3"/>
+      <c r="A140" s="9"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="3"/>
+      <c r="A141" s="9"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
@@ -3531,25 +3485,25 @@
       <c r="D147" s="8"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="9"/>
+      <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="9"/>
+      <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="9"/>
+      <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="9"/>
+      <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
@@ -3561,28 +3515,20 @@
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="3"/>
-      <c r="B153" s="4"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
+      <c r="A153" s="4"/>
+      <c r="B153" s="5"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="3"/>
-      <c r="B154" s="4"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
+      <c r="A154" s="4"/>
+      <c r="B154" s="5"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="3"/>
-      <c r="B155" s="4"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
+      <c r="A155" s="4"/>
+      <c r="B155" s="5"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="3"/>
-      <c r="B156" s="4"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
+      <c r="A156" s="4"/>
+      <c r="B156" s="5"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
@@ -3901,19 +3847,19 @@
       <c r="B235" s="5"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="4"/>
+      <c r="A236" s="3"/>
       <c r="B236" s="5"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="4"/>
+      <c r="A237" s="3"/>
       <c r="B237" s="5"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="4"/>
+      <c r="A238" s="3"/>
       <c r="B238" s="5"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="4"/>
+      <c r="A239" s="3"/>
       <c r="B239" s="5"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -3955,22 +3901,6 @@
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="3"/>
-      <c r="B250" s="5"/>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="3"/>
-      <c r="B251" s="5"/>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="3"/>
-      <c r="B252" s="5"/>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="3"/>
-      <c r="B253" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3979,6 +3909,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4219,7 +4158,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -4231,16 +4170,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4259,27 +4197,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update on KORA S1 and S3, P2
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666ACD5-488A-46B5-92B7-740638CFBDBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666ACD5-488A-46B5-92B7-740638CFBDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -21,6 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -40,6 +51,9 @@
     <t>valueType</t>
   </si>
   <si>
+    <t>A_ID</t>
+  </si>
+  <si>
     <t>ID of the participant</t>
   </si>
   <si>
@@ -695,16 +709,13 @@
   </si>
   <si>
     <t>unknown</t>
-  </si>
-  <si>
-    <t>A_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -801,7 +812,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -817,7 +828,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1119,7 +1130,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="9"/>
     <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -1127,7 +1138,7 @@
     <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1141,1421 +1152,1421 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="9">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>223</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="9">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="9">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="9">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="9">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="9">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="9">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="9">
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="9">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="9">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="9">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="9">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="9">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="9">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="9">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="9">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="9">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="9">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="9">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="9">
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="9">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="9">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="9">
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="9">
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="9">
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="9">
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="9">
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="9">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="9">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="9">
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="9">
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="9">
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="9">
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="9">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="9">
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="9">
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="9">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="9">
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="9">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="9">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="9">
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="9">
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="9">
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="9">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="9">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="9">
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="9">
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="9">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="9">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="9">
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="9">
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="9">
         <v>65</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="9">
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="9">
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="9">
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="9">
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="9">
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="9">
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="9">
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="9">
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="9">
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="9">
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="9">
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="9">
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="9">
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="9">
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" s="9">
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="9">
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" s="9">
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" s="9">
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" s="9">
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" s="9">
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="9">
         <v>86</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" s="9">
         <v>87</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" s="9">
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="9">
         <v>89</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" s="9">
         <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" s="9">
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F92" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" s="9">
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" s="9">
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" s="9">
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" s="9">
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="9">
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="9">
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="9">
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="9">
         <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="9">
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="9">
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2572,16 +2583,16 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2590,1385 +2601,1385 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="8" customFormat="1">
       <c r="A2" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1">
       <c r="A3" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1">
       <c r="A4" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="12">
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1">
       <c r="A5" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1">
       <c r="A6" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="12">
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1">
       <c r="A7" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="12">
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1">
       <c r="A8" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="12">
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1">
       <c r="A9" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="12">
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="12">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="12">
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="12">
         <v>3</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="12">
         <v>4</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4">
       <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4">
       <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2">
       <c r="A237" s="4"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2">
       <c r="A238" s="4"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2">
       <c r="A239" s="4"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2">
       <c r="A250" s="3"/>
       <c r="B250" s="5"/>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2">
       <c r="A251" s="3"/>
       <c r="B251" s="5"/>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2">
       <c r="A252" s="3"/>
       <c r="B252" s="5"/>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2">
       <c r="A253" s="3"/>
       <c r="B253" s="5"/>
     </row>
@@ -3979,6 +3990,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4219,67 +4251,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81CF8071-E6E9-4774-98D1-93B3A066C1B7}"/>
 </file>
</xml_diff>

<commit_message>
re-update P1 DD and DPE for main
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{355F4338-A502-405F-B1B3-778194FD8D2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666ACD5-488A-46B5-92B7-740638CFBDBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="224">
   <si>
     <t>index</t>
   </si>
@@ -43,6 +43,9 @@
     <t>ID of the participant</t>
   </si>
   <si>
+    <t>text</t>
+  </si>
+  <si>
     <t>acsex</t>
   </si>
   <si>
@@ -79,6 +82,12 @@
     <t>decimal</t>
   </si>
   <si>
+    <t>akcal</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
     <t>AV410</t>
   </si>
   <si>
@@ -640,6 +649,12 @@
     <t>fruit wine</t>
   </si>
   <si>
+    <t>AV491</t>
+  </si>
+  <si>
+    <t>dry legumes</t>
+  </si>
+  <si>
     <t>variable</t>
   </si>
   <si>
@@ -649,6 +664,15 @@
     <t>male</t>
   </si>
   <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>primary school completed</t>
+  </si>
+  <si>
     <t>technical/professional school completed</t>
   </si>
   <si>
@@ -658,6 +682,9 @@
     <t>longer education (incl. university)</t>
   </si>
   <si>
+    <t>not specified</t>
+  </si>
+  <si>
     <t>never</t>
   </si>
   <si>
@@ -667,29 +694,17 @@
     <t>current</t>
   </si>
   <si>
-    <t>a_id</t>
-  </si>
-  <si>
-    <t>AV491</t>
-  </si>
-  <si>
-    <t>dry legumes</t>
-  </si>
-  <si>
-    <t>primary school completed</t>
-  </si>
-  <si>
-    <t>akcal</t>
-  </si>
-  <si>
-    <t>energy</t>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>A_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,6 +733,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -739,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -774,6 +795,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1092,14 +1116,14 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="9"/>
+    <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
@@ -1122,13 +1146,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,13 +1160,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,13 +1174,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,13 +1188,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,13 +1202,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,27 +1216,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>217</v>
+      <c r="B8" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>218</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,13 +1244,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,13 +1258,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,13 +1272,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,13 +1286,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,13 +1300,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,13 +1314,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,13 +1328,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1318,13 +1342,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1332,13 +1356,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,13 +1370,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,13 +1384,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1374,13 +1398,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,27 +1412,27 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>214</v>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>215</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,13 +1440,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,13 +1454,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,13 +1468,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,13 +1482,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,13 +1496,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,13 +1510,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1500,13 +1524,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1514,13 +1538,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1528,13 +1552,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1542,13 +1566,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1556,13 +1580,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,13 +1594,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1584,13 +1608,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1598,27 +1622,27 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>72</v>
+      <c r="B37" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1626,27 +1650,27 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>75</v>
+      <c r="B39" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1654,13 +1678,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1668,13 +1692,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1682,13 +1706,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,13 +1720,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>84</v>
+        <v>88</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,13 +1734,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1724,13 +1748,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,13 +1762,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1752,13 +1776,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,13 +1790,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,13 +1804,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1794,13 +1818,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,13 +1832,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,13 +1846,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,13 +1860,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,13 +1874,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>106</v>
+        <v>110</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,13 +1888,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,13 +1902,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1892,13 +1916,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,13 +1930,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,13 +1944,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>116</v>
+        <v>120</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,13 +1958,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1948,13 +1972,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,13 +1986,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,13 +2000,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>124</v>
+        <v>128</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,13 +2014,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2004,27 +2028,27 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>130</v>
+      <c r="B66" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2032,13 +2056,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,13 +2070,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,13 +2084,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,13 +2098,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2088,13 +2112,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,13 +2126,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,13 +2140,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,13 +2154,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,13 +2168,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,13 +2182,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,13 +2196,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,13 +2210,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,13 +2224,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,13 +2238,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,13 +2252,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2242,13 +2266,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2256,27 +2280,27 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
-      <c r="B84" s="9" t="s">
-        <v>165</v>
+      <c r="B84" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2284,13 +2308,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2298,27 +2322,27 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
-      <c r="B87" s="3" t="s">
-        <v>171</v>
+      <c r="B87" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2326,41 +2350,41 @@
         <v>87</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>174</v>
+        <v>178</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
-      <c r="B89" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>176</v>
+      <c r="B89" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>177</v>
+      <c r="B90" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2368,13 +2392,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2382,13 +2406,16 @@
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F92" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2396,16 +2423,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F93" t="s">
-        <v>185</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2413,13 +2437,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2427,13 +2451,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2441,13 +2465,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2455,13 +2479,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2469,13 +2493,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,13 +2507,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,13 +2521,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,13 +2535,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2525,13 +2549,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2542,20 +2566,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
-  <dimension ref="A1:E249"/>
+  <dimension ref="A1:E253"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2564,121 +2590,141 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>216</v>
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="12">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="12">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="C8" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="12">
+        <v>5</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="12">
         <v>1</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="C10" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="12">
         <v>2</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="12">
+      <c r="C11" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12">
         <v>3</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="C12" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="12">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -2825,25 +2871,25 @@
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -3425,25 +3471,25 @@
       <c r="D137" s="8"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="9"/>
+      <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="9"/>
+      <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="9"/>
+      <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="9"/>
+      <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
@@ -3485,25 +3531,25 @@
       <c r="D147" s="8"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="3"/>
+      <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="3"/>
+      <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="3"/>
+      <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="3"/>
+      <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
@@ -3515,20 +3561,28 @@
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="4"/>
-      <c r="B153" s="5"/>
+      <c r="A153" s="3"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="4"/>
-      <c r="B154" s="5"/>
+      <c r="A154" s="3"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="4"/>
-      <c r="B155" s="5"/>
+      <c r="A155" s="3"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="4"/>
-      <c r="B156" s="5"/>
+      <c r="A156" s="3"/>
+      <c r="B156" s="4"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
@@ -3847,19 +3901,19 @@
       <c r="B235" s="5"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="3"/>
+      <c r="A236" s="4"/>
       <c r="B236" s="5"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="3"/>
+      <c r="A237" s="4"/>
       <c r="B237" s="5"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="3"/>
+      <c r="A238" s="4"/>
       <c r="B238" s="5"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="3"/>
+      <c r="A239" s="4"/>
       <c r="B239" s="5"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -3901,6 +3955,22 @@
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="3"/>
+      <c r="B250" s="5"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="3"/>
+      <c r="B251" s="5"/>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="3"/>
+      <c r="B252" s="5"/>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="3"/>
+      <c r="B253" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3909,15 +3979,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4158,7 +4219,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -4170,15 +4231,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4197,19 +4259,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating P1 files for main
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666ACD5-488A-46B5-92B7-740638CFBDBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{355F4338-A502-405F-B1B3-778194FD8D2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="219">
   <si>
     <t>index</t>
   </si>
@@ -43,9 +43,6 @@
     <t>ID of the participant</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>acsex</t>
   </si>
   <si>
@@ -82,629 +79,617 @@
     <t>decimal</t>
   </si>
   <si>
+    <t>AV410</t>
+  </si>
+  <si>
+    <t>potatoes</t>
+  </si>
+  <si>
+    <t>AV420</t>
+  </si>
+  <si>
+    <t>potato products</t>
+  </si>
+  <si>
+    <t>AV431</t>
+  </si>
+  <si>
+    <t>cauliflower</t>
+  </si>
+  <si>
+    <t>AV433</t>
+  </si>
+  <si>
+    <t>other cabbage</t>
+  </si>
+  <si>
+    <t>AV440</t>
+  </si>
+  <si>
+    <t>leafy and stem vegetables</t>
+  </si>
+  <si>
+    <t>AV451</t>
+  </si>
+  <si>
+    <t>tomatoes</t>
+  </si>
+  <si>
+    <t>AV455</t>
+  </si>
+  <si>
+    <t>cucumbers</t>
+  </si>
+  <si>
+    <t>AV459</t>
+  </si>
+  <si>
+    <t>other fruit vegetables</t>
+  </si>
+  <si>
+    <t>AV461</t>
+  </si>
+  <si>
+    <t>onion vegetables</t>
+  </si>
+  <si>
+    <t>AV465</t>
+  </si>
+  <si>
+    <t>carrots</t>
+  </si>
+  <si>
+    <t>AV469</t>
+  </si>
+  <si>
+    <t>other fresh vegetables</t>
+  </si>
+  <si>
+    <t>AV470</t>
+  </si>
+  <si>
+    <t>frozen vegetables</t>
+  </si>
+  <si>
+    <t>AV480</t>
+  </si>
+  <si>
+    <t>canned vegetables</t>
+  </si>
+  <si>
+    <t>AV499</t>
+  </si>
+  <si>
+    <t>other vegetable products</t>
+  </si>
+  <si>
+    <t>AV310</t>
+  </si>
+  <si>
+    <t>fruit without specification</t>
+  </si>
+  <si>
+    <t>AV311</t>
+  </si>
+  <si>
+    <t>apples</t>
+  </si>
+  <si>
+    <t>AV315</t>
+  </si>
+  <si>
+    <t>other pome fruits</t>
+  </si>
+  <si>
+    <t>AV321</t>
+  </si>
+  <si>
+    <t>peaches</t>
+  </si>
+  <si>
+    <t>AV323</t>
+  </si>
+  <si>
+    <t>cherries</t>
+  </si>
+  <si>
+    <t>AV325</t>
+  </si>
+  <si>
+    <t>other stone fruits</t>
+  </si>
+  <si>
+    <t>AV331</t>
+  </si>
+  <si>
+    <t>strawberries</t>
+  </si>
+  <si>
+    <t>AV334</t>
+  </si>
+  <si>
+    <t>other berries</t>
+  </si>
+  <si>
+    <t>AV337</t>
+  </si>
+  <si>
+    <t>grapes</t>
+  </si>
+  <si>
+    <t>AV341</t>
+  </si>
+  <si>
+    <t>oranges, mandarins</t>
+  </si>
+  <si>
+    <t>AV343</t>
+  </si>
+  <si>
+    <t>grapefruits</t>
+  </si>
+  <si>
+    <t>AV344</t>
+  </si>
+  <si>
+    <t>other citrus fruits</t>
+  </si>
+  <si>
+    <t>AV345</t>
+  </si>
+  <si>
+    <t>bananas</t>
+  </si>
+  <si>
+    <t>AV346</t>
+  </si>
+  <si>
+    <t>other tropical fruits</t>
+  </si>
+  <si>
+    <t>AV351</t>
+  </si>
+  <si>
+    <t>nuts</t>
+  </si>
+  <si>
+    <t>AV357</t>
+  </si>
+  <si>
+    <t>dried fruit</t>
+  </si>
+  <si>
+    <t>AV360</t>
+  </si>
+  <si>
+    <t>canned fruit</t>
+  </si>
+  <si>
+    <t>AV370</t>
+  </si>
+  <si>
+    <t>frozen fruit</t>
+  </si>
+  <si>
+    <t>AV390</t>
+  </si>
+  <si>
+    <t>other processed fruit</t>
+  </si>
+  <si>
+    <t>AV210</t>
+  </si>
+  <si>
+    <t>drinking milk</t>
+  </si>
+  <si>
+    <t>AV220</t>
+  </si>
+  <si>
+    <t>condensed milk or powder</t>
+  </si>
+  <si>
+    <t>AV231</t>
+  </si>
+  <si>
+    <t>cream</t>
+  </si>
+  <si>
+    <t>AV232</t>
+  </si>
+  <si>
+    <t>yogurt, soured milk</t>
+  </si>
+  <si>
+    <t>AV233</t>
+  </si>
+  <si>
+    <t>other dairy products</t>
+  </si>
+  <si>
+    <t>AV245</t>
+  </si>
+  <si>
+    <t>fresh cheese, curd</t>
+  </si>
+  <si>
+    <t>AV248</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>AV711</t>
+  </si>
+  <si>
+    <t>Wheat flour</t>
+  </si>
+  <si>
+    <t>AV715</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>AV731</t>
+  </si>
+  <si>
+    <t>Pasta</t>
+  </si>
+  <si>
+    <t>AV719</t>
+  </si>
+  <si>
+    <t>Products from other cereals</t>
+  </si>
+  <si>
+    <t>AV511</t>
+  </si>
+  <si>
+    <t>White bread</t>
+  </si>
+  <si>
+    <t>AV512</t>
+  </si>
+  <si>
+    <t>Brown bread</t>
+  </si>
+  <si>
+    <t>AV517</t>
+  </si>
+  <si>
+    <t>Other bread</t>
+  </si>
+  <si>
+    <t>AV515</t>
+  </si>
+  <si>
+    <t>Crisp bread</t>
+  </si>
+  <si>
+    <t>AV540</t>
+  </si>
+  <si>
+    <t>Fine bakery products</t>
+  </si>
+  <si>
+    <t>AV111</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>AV112</t>
+  </si>
+  <si>
+    <t>Veal</t>
+  </si>
+  <si>
+    <t>AV113</t>
+  </si>
+  <si>
+    <t>Pork meat</t>
+  </si>
+  <si>
+    <t>AV115</t>
+  </si>
+  <si>
+    <t>Sheep or goat meat</t>
+  </si>
+  <si>
+    <t>AV117</t>
+  </si>
+  <si>
+    <t>Game meat</t>
+  </si>
+  <si>
+    <t>AV119</t>
+  </si>
+  <si>
+    <t>other meat</t>
+  </si>
+  <si>
+    <t>AV120</t>
+  </si>
+  <si>
+    <t>Poultry meat</t>
+  </si>
+  <si>
+    <t>AV131</t>
+  </si>
+  <si>
+    <t>Minced meat</t>
+  </si>
+  <si>
+    <t>AV135</t>
+  </si>
+  <si>
+    <t>Animal offal</t>
+  </si>
+  <si>
+    <t>AV141</t>
+  </si>
+  <si>
+    <t>Sausage</t>
+  </si>
+  <si>
+    <t>AV145</t>
+  </si>
+  <si>
+    <t>Ham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV147 </t>
+  </si>
+  <si>
+    <t>Bacon</t>
+  </si>
+  <si>
+    <t>AV150</t>
+  </si>
+  <si>
+    <t>canned, frozen meat or meat products</t>
+  </si>
+  <si>
+    <t>AV160</t>
+  </si>
+  <si>
+    <t>other meat products</t>
+  </si>
+  <si>
+    <t>AV170</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>AV180</t>
+  </si>
+  <si>
+    <t>canned fish</t>
+  </si>
+  <si>
+    <t>AV190</t>
+  </si>
+  <si>
+    <t>other fish products</t>
+  </si>
+  <si>
+    <t>AV250</t>
+  </si>
+  <si>
+    <t>fresh eggs</t>
+  </si>
+  <si>
+    <t>AV255</t>
+  </si>
+  <si>
+    <t>egg products</t>
+  </si>
+  <si>
+    <t>AV270</t>
+  </si>
+  <si>
+    <t>butter</t>
+  </si>
+  <si>
+    <t>AV291</t>
+  </si>
+  <si>
+    <t>margarine</t>
+  </si>
+  <si>
+    <t>AV293</t>
+  </si>
+  <si>
+    <t>vegetable edible oils</t>
+  </si>
+  <si>
+    <t>AV295</t>
+  </si>
+  <si>
+    <t>other edible oils</t>
+  </si>
+  <si>
+    <t>AV610</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>AV681</t>
+  </si>
+  <si>
+    <t>Honey</t>
+  </si>
+  <si>
+    <t>AV684</t>
+  </si>
+  <si>
+    <t>Jam</t>
+  </si>
+  <si>
+    <t>AV687</t>
+  </si>
+  <si>
+    <t>Other sweet spreads</t>
+  </si>
+  <si>
+    <t>AV620</t>
+  </si>
+  <si>
+    <t>cacao products</t>
+  </si>
+  <si>
+    <t>AV630</t>
+  </si>
+  <si>
+    <t>chocolate products</t>
+  </si>
+  <si>
+    <t>AV650</t>
+  </si>
+  <si>
+    <t>confectionary</t>
+  </si>
+  <si>
+    <t>AV670</t>
+  </si>
+  <si>
+    <t>all ice cream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AV570 </t>
+  </si>
+  <si>
+    <t>long-life baked goods</t>
+  </si>
+  <si>
+    <t>AV810</t>
+  </si>
+  <si>
+    <t>fruit/vegetable juice</t>
+  </si>
+  <si>
+    <t>AV821</t>
+  </si>
+  <si>
+    <t>table water</t>
+  </si>
+  <si>
+    <t>AV825</t>
+  </si>
+  <si>
+    <t>caffeinated lemonade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AV829</t>
+  </si>
+  <si>
+    <t>other soft drinks</t>
+  </si>
+  <si>
+    <t>AV841</t>
+  </si>
+  <si>
+    <t>roasted coffee</t>
+  </si>
+  <si>
+    <t>AV845</t>
+  </si>
+  <si>
+    <t>coffee extracts</t>
+  </si>
+  <si>
+    <t>AV850</t>
+  </si>
+  <si>
+    <t>tea</t>
+  </si>
+  <si>
+    <t>AV860</t>
+  </si>
+  <si>
+    <t>spirits</t>
+  </si>
+  <si>
+    <t>AV870</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>AV881</t>
+  </si>
+  <si>
+    <t>grape wine</t>
+  </si>
+  <si>
+    <t>AV885</t>
+  </si>
+  <si>
+    <t>grape sparkling wine</t>
+  </si>
+  <si>
+    <t>AV889</t>
+  </si>
+  <si>
+    <t>fruit wine</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>technical/professional school completed</t>
+  </si>
+  <si>
+    <t>secondary school</t>
+  </si>
+  <si>
+    <t>longer education (incl. university)</t>
+  </si>
+  <si>
+    <t>never</t>
+  </si>
+  <si>
+    <t>former</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>a_id</t>
+  </si>
+  <si>
+    <t>AV491</t>
+  </si>
+  <si>
+    <t>dry legumes</t>
+  </si>
+  <si>
+    <t>primary school completed</t>
+  </si>
+  <si>
     <t>akcal</t>
   </si>
   <si>
     <t>energy</t>
-  </si>
-  <si>
-    <t>AV410</t>
-  </si>
-  <si>
-    <t>potatoes</t>
-  </si>
-  <si>
-    <t>AV420</t>
-  </si>
-  <si>
-    <t>potato products</t>
-  </si>
-  <si>
-    <t>AV431</t>
-  </si>
-  <si>
-    <t>cauliflower</t>
-  </si>
-  <si>
-    <t>AV433</t>
-  </si>
-  <si>
-    <t>other cabbage</t>
-  </si>
-  <si>
-    <t>AV440</t>
-  </si>
-  <si>
-    <t>leafy and stem vegetables</t>
-  </si>
-  <si>
-    <t>AV451</t>
-  </si>
-  <si>
-    <t>tomatoes</t>
-  </si>
-  <si>
-    <t>AV455</t>
-  </si>
-  <si>
-    <t>cucumbers</t>
-  </si>
-  <si>
-    <t>AV459</t>
-  </si>
-  <si>
-    <t>other fruit vegetables</t>
-  </si>
-  <si>
-    <t>AV461</t>
-  </si>
-  <si>
-    <t>onion vegetables</t>
-  </si>
-  <si>
-    <t>AV465</t>
-  </si>
-  <si>
-    <t>carrots</t>
-  </si>
-  <si>
-    <t>AV469</t>
-  </si>
-  <si>
-    <t>other fresh vegetables</t>
-  </si>
-  <si>
-    <t>AV470</t>
-  </si>
-  <si>
-    <t>frozen vegetables</t>
-  </si>
-  <si>
-    <t>AV480</t>
-  </si>
-  <si>
-    <t>canned vegetables</t>
-  </si>
-  <si>
-    <t>AV499</t>
-  </si>
-  <si>
-    <t>other vegetable products</t>
-  </si>
-  <si>
-    <t>AV310</t>
-  </si>
-  <si>
-    <t>fruit without specification</t>
-  </si>
-  <si>
-    <t>AV311</t>
-  </si>
-  <si>
-    <t>apples</t>
-  </si>
-  <si>
-    <t>AV315</t>
-  </si>
-  <si>
-    <t>other pome fruits</t>
-  </si>
-  <si>
-    <t>AV321</t>
-  </si>
-  <si>
-    <t>peaches</t>
-  </si>
-  <si>
-    <t>AV323</t>
-  </si>
-  <si>
-    <t>cherries</t>
-  </si>
-  <si>
-    <t>AV325</t>
-  </si>
-  <si>
-    <t>other stone fruits</t>
-  </si>
-  <si>
-    <t>AV331</t>
-  </si>
-  <si>
-    <t>strawberries</t>
-  </si>
-  <si>
-    <t>AV334</t>
-  </si>
-  <si>
-    <t>other berries</t>
-  </si>
-  <si>
-    <t>AV337</t>
-  </si>
-  <si>
-    <t>grapes</t>
-  </si>
-  <si>
-    <t>AV341</t>
-  </si>
-  <si>
-    <t>oranges, mandarins</t>
-  </si>
-  <si>
-    <t>AV343</t>
-  </si>
-  <si>
-    <t>grapefruits</t>
-  </si>
-  <si>
-    <t>AV344</t>
-  </si>
-  <si>
-    <t>other citrus fruits</t>
-  </si>
-  <si>
-    <t>AV345</t>
-  </si>
-  <si>
-    <t>bananas</t>
-  </si>
-  <si>
-    <t>AV346</t>
-  </si>
-  <si>
-    <t>other tropical fruits</t>
-  </si>
-  <si>
-    <t>AV351</t>
-  </si>
-  <si>
-    <t>nuts</t>
-  </si>
-  <si>
-    <t>AV357</t>
-  </si>
-  <si>
-    <t>dried fruit</t>
-  </si>
-  <si>
-    <t>AV360</t>
-  </si>
-  <si>
-    <t>canned fruit</t>
-  </si>
-  <si>
-    <t>AV370</t>
-  </si>
-  <si>
-    <t>frozen fruit</t>
-  </si>
-  <si>
-    <t>AV390</t>
-  </si>
-  <si>
-    <t>other processed fruit</t>
-  </si>
-  <si>
-    <t>AV210</t>
-  </si>
-  <si>
-    <t>drinking milk</t>
-  </si>
-  <si>
-    <t>AV220</t>
-  </si>
-  <si>
-    <t>condensed milk or powder</t>
-  </si>
-  <si>
-    <t>AV231</t>
-  </si>
-  <si>
-    <t>cream</t>
-  </si>
-  <si>
-    <t>AV232</t>
-  </si>
-  <si>
-    <t>yogurt, soured milk</t>
-  </si>
-  <si>
-    <t>AV233</t>
-  </si>
-  <si>
-    <t>other dairy products</t>
-  </si>
-  <si>
-    <t>AV245</t>
-  </si>
-  <si>
-    <t>fresh cheese, curd</t>
-  </si>
-  <si>
-    <t>AV248</t>
-  </si>
-  <si>
-    <t>cheese</t>
-  </si>
-  <si>
-    <t>AV711</t>
-  </si>
-  <si>
-    <t>Wheat flour</t>
-  </si>
-  <si>
-    <t>AV715</t>
-  </si>
-  <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>AV731</t>
-  </si>
-  <si>
-    <t>Pasta</t>
-  </si>
-  <si>
-    <t>AV719</t>
-  </si>
-  <si>
-    <t>Products from other cereals</t>
-  </si>
-  <si>
-    <t>AV511</t>
-  </si>
-  <si>
-    <t>White bread</t>
-  </si>
-  <si>
-    <t>AV512</t>
-  </si>
-  <si>
-    <t>Brown bread</t>
-  </si>
-  <si>
-    <t>AV517</t>
-  </si>
-  <si>
-    <t>Other bread</t>
-  </si>
-  <si>
-    <t>AV515</t>
-  </si>
-  <si>
-    <t>Crisp bread</t>
-  </si>
-  <si>
-    <t>AV540</t>
-  </si>
-  <si>
-    <t>Fine bakery products</t>
-  </si>
-  <si>
-    <t>AV111</t>
-  </si>
-  <si>
-    <t>Beef</t>
-  </si>
-  <si>
-    <t>AV112</t>
-  </si>
-  <si>
-    <t>Veal</t>
-  </si>
-  <si>
-    <t>AV113</t>
-  </si>
-  <si>
-    <t>Pork meat</t>
-  </si>
-  <si>
-    <t>AV115</t>
-  </si>
-  <si>
-    <t>Sheep or goat meat</t>
-  </si>
-  <si>
-    <t>AV117</t>
-  </si>
-  <si>
-    <t>Game meat</t>
-  </si>
-  <si>
-    <t>AV119</t>
-  </si>
-  <si>
-    <t>other meat</t>
-  </si>
-  <si>
-    <t>AV120</t>
-  </si>
-  <si>
-    <t>Poultry meat</t>
-  </si>
-  <si>
-    <t>AV131</t>
-  </si>
-  <si>
-    <t>Minced meat</t>
-  </si>
-  <si>
-    <t>AV135</t>
-  </si>
-  <si>
-    <t>Animal offal</t>
-  </si>
-  <si>
-    <t>AV141</t>
-  </si>
-  <si>
-    <t>Sausage</t>
-  </si>
-  <si>
-    <t>AV145</t>
-  </si>
-  <si>
-    <t>Ham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AV147 </t>
-  </si>
-  <si>
-    <t>Bacon</t>
-  </si>
-  <si>
-    <t>AV150</t>
-  </si>
-  <si>
-    <t>canned, frozen meat or meat products</t>
-  </si>
-  <si>
-    <t>AV160</t>
-  </si>
-  <si>
-    <t>other meat products</t>
-  </si>
-  <si>
-    <t>AV170</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-  <si>
-    <t>AV180</t>
-  </si>
-  <si>
-    <t>canned fish</t>
-  </si>
-  <si>
-    <t>AV190</t>
-  </si>
-  <si>
-    <t>other fish products</t>
-  </si>
-  <si>
-    <t>AV250</t>
-  </si>
-  <si>
-    <t>fresh eggs</t>
-  </si>
-  <si>
-    <t>AV255</t>
-  </si>
-  <si>
-    <t>egg products</t>
-  </si>
-  <si>
-    <t>AV270</t>
-  </si>
-  <si>
-    <t>butter</t>
-  </si>
-  <si>
-    <t>AV291</t>
-  </si>
-  <si>
-    <t>margarine</t>
-  </si>
-  <si>
-    <t>AV293</t>
-  </si>
-  <si>
-    <t>vegetable edible oils</t>
-  </si>
-  <si>
-    <t>AV295</t>
-  </si>
-  <si>
-    <t>other edible oils</t>
-  </si>
-  <si>
-    <t>AV610</t>
-  </si>
-  <si>
-    <t>sugar</t>
-  </si>
-  <si>
-    <t>AV681</t>
-  </si>
-  <si>
-    <t>Honey</t>
-  </si>
-  <si>
-    <t>AV684</t>
-  </si>
-  <si>
-    <t>Jam</t>
-  </si>
-  <si>
-    <t>AV687</t>
-  </si>
-  <si>
-    <t>Other sweet spreads</t>
-  </si>
-  <si>
-    <t>AV620</t>
-  </si>
-  <si>
-    <t>cacao products</t>
-  </si>
-  <si>
-    <t>AV630</t>
-  </si>
-  <si>
-    <t>chocolate products</t>
-  </si>
-  <si>
-    <t>AV650</t>
-  </si>
-  <si>
-    <t>confectionary</t>
-  </si>
-  <si>
-    <t>AV670</t>
-  </si>
-  <si>
-    <t>all ice cream</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AV570 </t>
-  </si>
-  <si>
-    <t>long-life baked goods</t>
-  </si>
-  <si>
-    <t>AV810</t>
-  </si>
-  <si>
-    <t>fruit/vegetable juice</t>
-  </si>
-  <si>
-    <t>AV821</t>
-  </si>
-  <si>
-    <t>table water</t>
-  </si>
-  <si>
-    <t>AV825</t>
-  </si>
-  <si>
-    <t>caffeinated lemonade</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>AV829</t>
-  </si>
-  <si>
-    <t>other soft drinks</t>
-  </si>
-  <si>
-    <t>AV841</t>
-  </si>
-  <si>
-    <t>roasted coffee</t>
-  </si>
-  <si>
-    <t>AV845</t>
-  </si>
-  <si>
-    <t>coffee extracts</t>
-  </si>
-  <si>
-    <t>AV850</t>
-  </si>
-  <si>
-    <t>tea</t>
-  </si>
-  <si>
-    <t>AV860</t>
-  </si>
-  <si>
-    <t>spirits</t>
-  </si>
-  <si>
-    <t>AV870</t>
-  </si>
-  <si>
-    <t>beer</t>
-  </si>
-  <si>
-    <t>AV881</t>
-  </si>
-  <si>
-    <t>grape wine</t>
-  </si>
-  <si>
-    <t>AV885</t>
-  </si>
-  <si>
-    <t>grape sparkling wine</t>
-  </si>
-  <si>
-    <t>AV889</t>
-  </si>
-  <si>
-    <t>fruit wine</t>
-  </si>
-  <si>
-    <t>AV491</t>
-  </si>
-  <si>
-    <t>dry legumes</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>primary school completed</t>
-  </si>
-  <si>
-    <t>technical/professional school completed</t>
-  </si>
-  <si>
-    <t>secondary school</t>
-  </si>
-  <si>
-    <t>longer education (incl. university)</t>
-  </si>
-  <si>
-    <t>not specified</t>
-  </si>
-  <si>
-    <t>never</t>
-  </si>
-  <si>
-    <t>former</t>
-  </si>
-  <si>
-    <t>current</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>A_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,12 +718,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -760,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,9 +774,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,14 +1092,14 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="9"/>
-    <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="9" style="9" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="9" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
@@ -1146,13 +1122,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,13 +1136,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1174,13 +1150,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,13 +1164,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,13 +1178,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,27 +1192,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>18</v>
+      <c r="B8" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>218</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,13 +1220,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,13 +1234,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,13 +1248,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,13 +1262,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,13 +1276,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,13 +1290,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,13 +1304,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,13 +1318,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,13 +1332,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,13 +1346,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,13 +1360,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,13 +1374,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,27 +1388,27 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+      <c r="B22" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,13 +1416,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,13 +1430,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1468,13 +1444,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,13 +1458,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1496,13 +1472,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,13 +1486,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1524,13 +1500,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1538,13 +1514,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,13 +1528,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,13 +1542,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1580,13 +1556,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1594,13 +1570,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,13 +1584,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1622,27 +1598,27 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>77</v>
+      <c r="B37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,27 +1626,27 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>80</v>
+      <c r="B39" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1678,13 +1654,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1692,13 +1668,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1706,13 +1682,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,13 +1696,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,13 +1710,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,13 +1724,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1762,13 +1738,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1776,13 +1752,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,13 +1766,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1804,13 +1780,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1818,13 +1794,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1832,13 +1808,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1846,13 +1822,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1860,13 +1836,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1874,13 +1850,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,13 +1864,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,13 +1878,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,13 +1892,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,13 +1906,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1944,13 +1920,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1958,13 +1934,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>123</v>
+        <v>117</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,13 +1948,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1986,13 +1962,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2000,13 +1976,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,13 +1990,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,27 +2004,27 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
-      <c r="B66" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>135</v>
+      <c r="B66" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2056,13 +2032,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2070,13 +2046,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,13 +2060,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2098,13 +2074,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,13 +2088,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,13 +2102,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2140,13 +2116,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,13 +2130,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2168,13 +2144,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2182,13 +2158,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2196,13 +2172,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2210,13 +2186,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,13 +2200,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2238,13 +2214,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2252,13 +2228,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2266,13 +2242,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2280,27 +2256,27 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>170</v>
+      <c r="B84" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2308,13 +2284,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2322,27 +2298,27 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
-      <c r="B87" s="9" t="s">
-        <v>176</v>
+      <c r="B87" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2350,41 +2326,41 @@
         <v>87</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>181</v>
+      <c r="B89" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
-      <c r="B90" s="9" t="s">
-        <v>182</v>
+      <c r="B90" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2392,13 +2368,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2406,16 +2382,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F92" t="s">
-        <v>188</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2423,13 +2396,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="F93" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2437,13 +2413,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2451,13 +2427,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2465,13 +2441,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2479,13 +2455,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2493,13 +2469,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2507,13 +2483,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2521,13 +2497,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2535,13 +2511,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2549,13 +2525,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2566,22 +2542,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2590,141 +2564,121 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>212</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="12">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="C8" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="12">
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="12">
-        <v>4</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="12">
-        <v>5</v>
-      </c>
       <c r="C9" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="12">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="12">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="12">
-        <v>4</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>222</v>
-      </c>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -2871,25 +2825,25 @@
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
+      <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+      <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+      <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+      <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -3471,25 +3425,25 @@
       <c r="D137" s="8"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="3"/>
+      <c r="A138" s="9"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="3"/>
+      <c r="A139" s="9"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="3"/>
+      <c r="A140" s="9"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="3"/>
+      <c r="A141" s="9"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
@@ -3531,25 +3485,25 @@
       <c r="D147" s="8"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="9"/>
+      <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="9"/>
+      <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="9"/>
+      <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="9"/>
+      <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
@@ -3561,28 +3515,20 @@
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="3"/>
-      <c r="B153" s="4"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
+      <c r="A153" s="4"/>
+      <c r="B153" s="5"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="3"/>
-      <c r="B154" s="4"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
+      <c r="A154" s="4"/>
+      <c r="B154" s="5"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="3"/>
-      <c r="B155" s="4"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
+      <c r="A155" s="4"/>
+      <c r="B155" s="5"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="3"/>
-      <c r="B156" s="4"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
+      <c r="A156" s="4"/>
+      <c r="B156" s="5"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
@@ -3901,19 +3847,19 @@
       <c r="B235" s="5"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="4"/>
+      <c r="A236" s="3"/>
       <c r="B236" s="5"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="4"/>
+      <c r="A237" s="3"/>
       <c r="B237" s="5"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="4"/>
+      <c r="A238" s="3"/>
       <c r="B238" s="5"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="4"/>
+      <c r="A239" s="3"/>
       <c r="B239" s="5"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -3955,22 +3901,6 @@
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" s="3"/>
-      <c r="B250" s="5"/>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="3"/>
-      <c r="B251" s="5"/>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" s="3"/>
-      <c r="B252" s="5"/>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="3"/>
-      <c r="B253" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3979,6 +3909,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4219,7 +4158,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -4231,16 +4170,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4259,27 +4197,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changing integer ages into decimal ages & tobacco_d into decimals
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{355F4338-A502-405F-B1B3-778194FD8D2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219AEEB9-11C1-4AF1-8AAA-15BD2E4B7382}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -1092,18 +1092,18 @@
   <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="9"/>
+    <col min="2" max="2" width="23.109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1156,10 +1156,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="9">
         <v>101</v>
       </c>
@@ -2546,14 +2546,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>204</v>
       </c>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2656,1249 +2656,1249 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="9"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="9"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="9"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="9"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="4"/>
       <c r="B153" s="5"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="4"/>
       <c r="B154" s="5"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="4"/>
       <c r="B155" s="5"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="4"/>
       <c r="B156" s="5"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="3"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="3"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="3"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="3"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>

</xml_diff>

<commit_message>
added category 4 of SMOKE_ST to the DD
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219AEEB9-11C1-4AF1-8AAA-15BD2E4B7382}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D385B0-DC86-495C-99EA-E3CAFFA05B6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="220">
   <si>
     <t>index</t>
   </si>
@@ -683,6 +683,9 @@
   </si>
   <si>
     <t>energy</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -1091,19 +1094,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="9"/>
+    <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1551,7 +1554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2377,7 +2380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2450,7 +2453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>101</v>
       </c>
@@ -2544,16 +2547,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>204</v>
       </c>
@@ -2568,7 +2573,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -2579,7 +2584,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -2590,7 +2595,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -2601,7 +2606,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -2612,7 +2617,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -2623,7 +2628,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2634,7 +2639,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -2645,7 +2650,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2656,1249 +2661,1255 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>219</v>
+      </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="9"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="9"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="9"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="9"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="B153" s="5"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="4"/>
       <c r="B154" s="5"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
       <c r="B155" s="5"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
       <c r="B156" s="5"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="3"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
@@ -3918,6 +3929,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4158,18 +4181,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -4179,6 +4190,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4195,21 +4223,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed smoking status categories to align with our definition (4 categories)
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219AEEB9-11C1-4AF1-8AAA-15BD2E4B7382}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E59E8E-2014-461E-AB31-7A3CC8029527}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="220">
   <si>
     <t>index</t>
   </si>
@@ -683,6 +683,9 @@
   </si>
   <si>
     <t>energy</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -1091,19 +1094,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.5546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="9"/>
+    <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1551,7 +1554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2377,7 +2380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2450,7 +2453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>101</v>
       </c>
@@ -2544,16 +2547,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:E249"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>204</v>
       </c>
@@ -2568,7 +2573,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -2579,7 +2584,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -2590,7 +2595,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -2601,7 +2606,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -2612,7 +2617,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -2623,7 +2628,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2631,10 +2636,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -2645,7 +2650,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2653,1252 +2658,1258 @@
         <v>3</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>219</v>
+      </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="9"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="9"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="9"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="9"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="B153" s="5"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="4"/>
       <c r="B154" s="5"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
       <c r="B155" s="5"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
       <c r="B156" s="5"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="3"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
@@ -3918,6 +3929,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4158,18 +4181,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -4179,6 +4190,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4195,21 +4223,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KORA-4 changes to DD_KORA_S1_P1 + DD_KORA_S1_P2 in atbbild and acsex categories and DD_KORA_S3_P1 + DD_KORA_S3_P2 in dcsex and dtbbild categories. Also, updated label of AV131 in DD_KORA_S1_P2 to match P1.
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E59E8E-2014-461E-AB31-7A3CC8029527}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2A35A8-FD7E-4846-A79C-743AFD05EBF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="222">
   <si>
     <t>index</t>
   </si>
@@ -686,6 +686,12 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>not specified</t>
   </si>
 </sst>
 </file>
@@ -780,7 +786,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -796,7 +802,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1094,11 +1100,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
@@ -2545,13 +2551,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
-  <dimension ref="A1:E249"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -2589,21 +2595,21 @@
         <v>10</v>
       </c>
       <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>216</v>
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="12">
-        <v>2</v>
+      <c r="B4" s="6">
+        <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2611,10 +2617,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2622,32 +2628,32 @@
         <v>10</v>
       </c>
       <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="12">
-        <v>1</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
+      <c r="A8" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -2655,34 +2661,44 @@
         <v>12</v>
       </c>
       <c r="B9" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="12">
+        <v>2</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12">
+        <v>3</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="12">
         <v>4</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2836,13 +2852,13 @@
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -3436,13 +3452,13 @@
       <c r="D137" s="8"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="9"/>
+      <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="9"/>
+      <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
@@ -3496,13 +3512,13 @@
       <c r="D147" s="8"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="3"/>
+      <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="3"/>
+      <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
@@ -3526,12 +3542,16 @@
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="4"/>
-      <c r="B153" s="5"/>
+      <c r="A153" s="3"/>
+      <c r="B153" s="4"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="4"/>
-      <c r="B154" s="5"/>
+      <c r="A154" s="3"/>
+      <c r="B154" s="4"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
@@ -3858,11 +3878,11 @@
       <c r="B235" s="5"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A236" s="3"/>
+      <c r="A236" s="4"/>
       <c r="B236" s="5"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A237" s="3"/>
+      <c r="A237" s="4"/>
       <c r="B237" s="5"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3912,6 +3932,14 @@
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="3"/>
+      <c r="B250" s="5"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="3"/>
+      <c r="B251" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3920,15 +3948,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -3940,7 +3959,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4181,15 +4200,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4206,7 +4226,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4223,4 +4243,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KORA-5 rearranged KORA education variable for all four (S1/S3 and P1/P2) harmonisation procedures to the original questions, added new mock data files and comparable files. Change to SAS file import needs to be still done after final check + check if caps for variable syntax is correct
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2A35A8-FD7E-4846-A79C-743AFD05EBF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BAADD7-C06E-4359-8D04-AD3B8ADF2803}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="227">
   <si>
     <t>index</t>
   </si>
@@ -58,12 +58,6 @@
     <t xml:space="preserve">age </t>
   </si>
   <si>
-    <t>atbbild</t>
-  </si>
-  <si>
-    <t>level of education</t>
-  </si>
-  <si>
     <t>atcigsmk</t>
   </si>
   <si>
@@ -649,15 +643,6 @@
     <t>male</t>
   </si>
   <si>
-    <t>technical/professional school completed</t>
-  </si>
-  <si>
-    <t>secondary school</t>
-  </si>
-  <si>
-    <t>longer education (incl. university)</t>
-  </si>
-  <si>
     <t>never</t>
   </si>
   <si>
@@ -676,9 +661,6 @@
     <t>dry legumes</t>
   </si>
   <si>
-    <t>primary school completed</t>
-  </si>
-  <si>
     <t>akcal</t>
   </si>
   <si>
@@ -688,17 +670,50 @@
     <t>unknown</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>not specified</t>
+    <t>AI13ABSC</t>
+  </si>
+  <si>
+    <t>highest school or university degree</t>
+  </si>
+  <si>
+    <t>AI14ABSC</t>
+  </si>
+  <si>
+    <t>highest vocational degree</t>
+  </si>
+  <si>
+    <t>Hauptschule/Volksschule</t>
+  </si>
+  <si>
+    <t>Mittlere Reife/Realschule</t>
+  </si>
+  <si>
+    <t>Abitur/Fachabitur</t>
+  </si>
+  <si>
+    <t>Hochschule/Fachhochschule/Universität</t>
+  </si>
+  <si>
+    <t>sonstiger Abschluss</t>
+  </si>
+  <si>
+    <t>kein Abschluss</t>
+  </si>
+  <si>
+    <t>Berufsschule (Lehre)</t>
+  </si>
+  <si>
+    <t>Fachschule/Techniker-/Meisterschule</t>
+  </si>
+  <si>
+    <t>Ingenieur-Schule/Polytechnikum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,6 +742,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -748,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -784,9 +805,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -802,7 +824,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1098,13 +1120,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="9" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="9" customWidth="1"/>
@@ -1131,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -1165,18 +1187,18 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
+      <c r="B5" s="13" t="s">
+        <v>214</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>215</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -1186,11 +1208,11 @@
       <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
+      <c r="B6" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>217</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -1201,13 +1223,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1215,13 +1237,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>217</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>218</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1229,13 +1251,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>211</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1243,13 +1265,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1257,13 +1279,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1271,13 +1293,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,13 +1307,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1299,13 +1321,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1313,13 +1335,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1327,27 +1349,27 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>34</v>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1355,13 +1377,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1369,13 +1391,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1383,27 +1405,27 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>41</v>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,27 +1433,27 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>214</v>
+        <v>39</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>215</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>43</v>
+      <c r="B23" s="9" t="s">
+        <v>209</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,13 +1461,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1453,13 +1475,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1467,13 +1489,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1481,13 +1503,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,13 +1517,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1509,13 +1531,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1523,13 +1545,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1537,13 +1559,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1551,13 +1573,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1565,13 +1587,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1579,13 +1601,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1593,13 +1615,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1607,13 +1629,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1621,27 +1643,27 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>74</v>
+      <c r="B38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1649,27 +1671,27 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>77</v>
+      <c r="B40" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1677,13 +1699,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1691,13 +1713,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,13 +1727,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1719,13 +1741,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1733,13 +1755,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1747,13 +1769,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1761,13 +1783,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1775,13 +1797,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,13 +1811,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1803,13 +1825,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,13 +1839,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1831,13 +1853,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1845,13 +1867,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1859,13 +1881,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1873,13 +1895,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,13 +1909,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1901,13 +1923,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1915,13 +1937,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1929,13 +1951,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1943,13 +1965,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1957,13 +1979,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1971,13 +1993,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,13 +2007,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1999,13 +2021,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2013,13 +2035,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2027,27 +2049,27 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>66</v>
       </c>
-      <c r="B67" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="9" t="s">
-        <v>132</v>
+      <c r="B67" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2055,13 +2077,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2069,13 +2091,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2083,13 +2105,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,13 +2119,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2111,13 +2133,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2125,13 +2147,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2139,13 +2161,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,13 +2175,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2167,13 +2189,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2181,13 +2203,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2195,13 +2217,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2209,13 +2231,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2223,13 +2245,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,13 +2259,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2251,13 +2273,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2265,13 +2287,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,27 +2301,27 @@
         <v>83</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>84</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>167</v>
+      <c r="B85" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,13 +2329,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2321,27 +2343,27 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>87</v>
       </c>
-      <c r="B88" s="9" t="s">
-        <v>173</v>
+      <c r="B88" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2349,41 +2371,41 @@
         <v>88</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>172</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>178</v>
+      <c r="B90" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>90</v>
       </c>
-      <c r="B91" s="9" t="s">
-        <v>179</v>
+      <c r="B91" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2391,13 +2413,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2405,16 +2427,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F93" t="s">
-        <v>185</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2422,13 +2441,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="F94" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2436,13 +2458,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2450,13 +2472,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,13 +2486,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2478,13 +2500,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2492,13 +2514,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2506,13 +2528,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2520,13 +2542,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2534,13 +2556,27 @@
         <v>101</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="9">
+        <v>102</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2551,13 +2587,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -2566,7 +2602,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2575,7 +2611,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -2587,154 +2623,184 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="6">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="6">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="6">
+        <v>4</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="6">
+        <v>5</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="12">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="17" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="B17" s="12">
+        <v>3</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="12">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="12">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="B18" s="12">
         <v>4</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="12">
-        <v>5</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="12">
-        <v>1</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="12">
-        <v>2</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="12">
-        <v>3</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="12">
-        <v>4</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="12" t="s">
+        <v>213</v>
+      </c>
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2864,37 +2930,37 @@
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -3464,37 +3530,37 @@
       <c r="D139" s="8"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="9"/>
+      <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="9"/>
+      <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="9"/>
+      <c r="A142" s="3"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="9"/>
+      <c r="A143" s="3"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="9"/>
+      <c r="A144" s="3"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="9"/>
+      <c r="A145" s="3"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
@@ -3524,58 +3590,70 @@
       <c r="D149" s="8"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="3"/>
+      <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="3"/>
+      <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="3"/>
+      <c r="A152" s="9"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="3"/>
+      <c r="A153" s="9"/>
       <c r="B153" s="4"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="3"/>
+      <c r="A154" s="9"/>
       <c r="B154" s="4"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="4"/>
-      <c r="B155" s="5"/>
+      <c r="A155" s="9"/>
+      <c r="B155" s="4"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="4"/>
-      <c r="B156" s="5"/>
+      <c r="A156" s="3"/>
+      <c r="B156" s="4"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="4"/>
-      <c r="B157" s="5"/>
+      <c r="A157" s="3"/>
+      <c r="B157" s="4"/>
+      <c r="C157" s="8"/>
+      <c r="D157" s="8"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="4"/>
-      <c r="B158" s="5"/>
+      <c r="A158" s="3"/>
+      <c r="B158" s="4"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="4"/>
-      <c r="B159" s="5"/>
+      <c r="A159" s="3"/>
+      <c r="B159" s="4"/>
+      <c r="C159" s="8"/>
+      <c r="D159" s="8"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="4"/>
-      <c r="B160" s="5"/>
+      <c r="A160" s="3"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="8"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
@@ -3886,27 +3964,27 @@
       <c r="B237" s="5"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A238" s="3"/>
+      <c r="A238" s="4"/>
       <c r="B238" s="5"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A239" s="3"/>
+      <c r="A239" s="4"/>
       <c r="B239" s="5"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" s="3"/>
+      <c r="A240" s="4"/>
       <c r="B240" s="5"/>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A241" s="3"/>
+      <c r="A241" s="4"/>
       <c r="B241" s="5"/>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" s="3"/>
+      <c r="A242" s="4"/>
       <c r="B242" s="5"/>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" s="3"/>
+      <c r="A243" s="4"/>
       <c r="B243" s="5"/>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3940,6 +4018,30 @@
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="3"/>
       <c r="B251" s="5"/>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="3"/>
+      <c r="B252" s="5"/>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="3"/>
+      <c r="B253" s="5"/>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="3"/>
+      <c r="B254" s="5"/>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="3"/>
+      <c r="B255" s="5"/>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="3"/>
+      <c r="B256" s="5"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="3"/>
+      <c r="B257" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3948,15 +4050,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4201,27 +4300,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4246,9 +4339,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KORA-5 changing education variable names input to lowercase according to e-mail exchange with data manager + tested for correct algorithm with defined data set + corrected some harmonisation status entries
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S1_P1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BAADD7-C06E-4359-8D04-AD3B8ADF2803}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73C8B14-70CD-4B22-B5C4-FF31D4CF6296}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -670,15 +670,9 @@
     <t>unknown</t>
   </si>
   <si>
-    <t>AI13ABSC</t>
-  </si>
-  <si>
     <t>highest school or university degree</t>
   </si>
   <si>
-    <t>AI14ABSC</t>
-  </si>
-  <si>
     <t>highest vocational degree</t>
   </si>
   <si>
@@ -707,6 +701,12 @@
   </si>
   <si>
     <t>Ingenieur-Schule/Polytechnikum</t>
+  </si>
+  <si>
+    <t>ai13absc</t>
+  </si>
+  <si>
+    <t>ai14absc</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,10 +1195,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -1209,10 +1209,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -2589,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:E257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,134 +2628,134 @@
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B6" s="6">
         <v>4</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B7" s="6">
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="B8" s="6">
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B9" s="12">
         <v>0</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B10" s="6">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B11" s="6">
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B12" s="6">
         <v>3</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B13" s="6">
         <v>4</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="B14" s="6">
         <v>5</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4050,15 +4050,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4299,6 +4290,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4312,14 +4312,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4334,6 +4326,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>